<commit_message>
added test cases and bug
</commit_message>
<xml_diff>
--- a/функциональное тестирование проект Дом питомца.xlsx
+++ b/функциональное тестирование проект Дом питомца.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="110" windowWidth="15120" windowHeight="8010"/>
+    <workbookView xWindow="120" yWindow="110" windowWidth="15120" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="чек-лист" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="224">
   <si>
     <r>
       <t xml:space="preserve">Функциональное тестирование сайта "Дом питомца": </t>
@@ -287,6 +287,450 @@
   </si>
   <si>
     <t>71.Оценка производительности и возможности оптимизации сайта "Дом питомца" на https://pagespeed.web.dev</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Precondition</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>EXP-001</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Главная страница сайта (Шапка)</t>
+  </si>
+  <si>
+    <t>1.Открыть страницу сайта http://130.193.37.179/app/pets</t>
+  </si>
+  <si>
+    <t>Открыта главная страница сайта. В шапке корректно отображаются пункты: "О нас","Питомцы", "Контакты", Так же отображается поиск: "Найти питомца".</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>EXP-002</t>
+  </si>
+  <si>
+    <t>Главная страница сайта (Тело)</t>
+  </si>
+  <si>
+    <t>Открыта главная страница сайта. В теле корректно отображается меню фильтра и сортировки. Так же внизу отображаются карточки питомцев с их данными и статусом: "хотят забрать" и "без дома" и порядковый номер страницы.</t>
+  </si>
+  <si>
+    <t>EXP-003</t>
+  </si>
+  <si>
+    <t>Главная страница сайта (Подвал)</t>
+  </si>
+  <si>
+    <t>Открыта главная страница сайта. В подвле корректно отображается "лого" сайта, а так же 4 кнопки для перехода в соц. Сети (Instagram, TikTok, YouTube, Telegram).</t>
+  </si>
+  <si>
+    <t>EXP-004</t>
+  </si>
+  <si>
+    <t>Страница "О нас" в шапке сайта</t>
+  </si>
+  <si>
+    <t>Открыта страница сайта http://130.193.37.179/app/pets</t>
+  </si>
+  <si>
+    <t>1.В навигации сайта кликнуть слева кнопку "О нас"</t>
+  </si>
+  <si>
+    <t>Корректно отображается описание приюта.Описание сайта соответствует предназначению сайта. "Шапка" и "Подвал" сайта остались без изменений.</t>
+  </si>
+  <si>
+    <t>EXP-005</t>
+  </si>
+  <si>
+    <t>Страница "Контакты" в шапке сайта</t>
+  </si>
+  <si>
+    <t>1.В навигации сайта кликнуть слева кнопку "Контакты"</t>
+  </si>
+  <si>
+    <t>Корректно отображается контактные данные приюта. "Шапка" и "Подвал" сайта остались без изменений</t>
+  </si>
+  <si>
+    <t>EXP-006</t>
+  </si>
+  <si>
+    <t>Страница "Питомцы" в шапке сайта</t>
+  </si>
+  <si>
+    <t>1.В "Шапке" сайта кликнуть слева кнопку "Питомцы"</t>
+  </si>
+  <si>
+    <t>Корректно отображается навигация. "Шапка" и "Подвал" сайта остались без изменений. Карточки питомцев,поиск и фильтр отображается и функционирует.</t>
+  </si>
+  <si>
+    <t>EXP-007</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Кнопка "Без дома"</t>
+  </si>
+  <si>
+    <t>1.Кликнуть на кнопку "Без дома"</t>
+  </si>
+  <si>
+    <t>При нажатии на кнопку "Без дома" выпадает всплывающее окно с вводом данных.</t>
+  </si>
+  <si>
+    <t>EXP-008</t>
+  </si>
+  <si>
+    <t>Кнопка "Хотят забрать"</t>
+  </si>
+  <si>
+    <t>1.Кликнуть на кнопку "Хотят забрать" в карточке питомца.</t>
+  </si>
+  <si>
+    <t>При нажатии на "Хотят забрать" выпадает всплывающее окно,с надписью" питомца хотят забрать,выберите другого или свяжитесь с нами"</t>
+  </si>
+  <si>
+    <t>Fail Bugs: FB-001</t>
+  </si>
+  <si>
+    <t>EXP-009</t>
+  </si>
+  <si>
+    <t>Кнопка "Питомцы без дома"</t>
+  </si>
+  <si>
+    <t>1.Кликнуть на кнопку "Питомцы без дома" над панелью фильтра</t>
+  </si>
+  <si>
+    <t>При нажатии на кнопку "Питомцы без дома" появляются все питомцы без дома в данный момент.</t>
+  </si>
+  <si>
+    <t>Fail Bugs: FB-002</t>
+  </si>
+  <si>
+    <t>EXP-010</t>
+  </si>
+  <si>
+    <t>Фильтр поиска
+(основная страница)</t>
+  </si>
+  <si>
+    <t>1. Кликнуть на кнопку поиска в "Шапке" страницы 2. Ввести "барон" 3. Нажать "Enter"</t>
+  </si>
+  <si>
+    <t>При введении "барон" и нажатии кнопки ENTER сайт автоматически находит карточку животного.</t>
+  </si>
+  <si>
+    <t>Fail Bugs: FB-003</t>
+  </si>
+  <si>
+    <t>EXP-011</t>
+  </si>
+  <si>
+    <t>Фильтр поиска
+(страница "контакты")</t>
+  </si>
+  <si>
+    <t>1. Кликнуть на кнопку "контакты",
+2. кликнуть на строку поиска в "Шапке" страницы 
+3. Ввести "барон" 
+4. Нажать "Enter"</t>
+  </si>
+  <si>
+    <t>Fail Bugs: FB-004</t>
+  </si>
+  <si>
+    <t>EXP-012</t>
+  </si>
+  <si>
+    <t>Кнопка "Счастливчики"</t>
+  </si>
+  <si>
+    <t>1.Кликнуть на кнопку "Счастливчики" над панелью фильтра</t>
+  </si>
+  <si>
+    <t>При нажатии на кнопку "Счастливчики" появляется отображение карточек питомца, которых уже приютили.</t>
+  </si>
+  <si>
+    <t>Fail Bugs: FB-005</t>
+  </si>
+  <si>
+    <t>EXP-013</t>
+  </si>
+  <si>
+    <t>Кнопка "Instagram"</t>
+  </si>
+  <si>
+    <t>1.Кликнуть по кнопке "Instagram" в "Подвале" сайта</t>
+  </si>
+  <si>
+    <t>Происходит переход в соцсеть "Instagram"</t>
+  </si>
+  <si>
+    <t>Fail Bugs: FB-006</t>
+  </si>
+  <si>
+    <t>EXP-014</t>
+  </si>
+  <si>
+    <t>Кнопка "TikTok"</t>
+  </si>
+  <si>
+    <t>1.Кликнуть по кнопке "TikTok" в "Подвале" сайта</t>
+  </si>
+  <si>
+    <t>Происходит переход в соцсеть "TikTok"</t>
+  </si>
+  <si>
+    <t>Fail Bugs: FB-007</t>
+  </si>
+  <si>
+    <t>EXP-015</t>
+  </si>
+  <si>
+    <t>Кнопка "YouTube"</t>
+  </si>
+  <si>
+    <t>1.Кликнуть по кнопке "YouTube" в "Подвале" сайта</t>
+  </si>
+  <si>
+    <t>Происходит переход в соцсеть "YouTube"</t>
+  </si>
+  <si>
+    <t>Fail Bugs: FB-008</t>
+  </si>
+  <si>
+    <t>EXP-016</t>
+  </si>
+  <si>
+    <t>Кнопка "Telegram"</t>
+  </si>
+  <si>
+    <t>1.Кликнуть по кнопке "Telegram" в "Подвале" сайта</t>
+  </si>
+  <si>
+    <t>Происходит переход в соцсеть "Telegram"</t>
+  </si>
+  <si>
+    <t>Fail Bugs: FB-009</t>
+  </si>
+  <si>
+    <t>EXP-017</t>
+  </si>
+  <si>
+    <t>Фильтр "вид животного"</t>
+  </si>
+  <si>
+    <t>1.Кликнуть по фильтру вид животного.</t>
+  </si>
+  <si>
+    <t>Открывается выпадающий список, в котором корректно указаны виды животных без деления на пол и без повторяющихся видов.</t>
+  </si>
+  <si>
+    <t>Fail Bugs: FB-0010</t>
+  </si>
+  <si>
+    <t>EXP-018</t>
+  </si>
+  <si>
+    <t>Фильтр "порода"</t>
+  </si>
+  <si>
+    <t>1.Кликнуть по фильтру порода.</t>
+  </si>
+  <si>
+    <t>Открывается выпадающий список, в котором корректно указаны породы животных без деления на пол и без повторяющихся видов.</t>
+  </si>
+  <si>
+    <t>1.Кликнуть по фильтру порода.
+2.Кликнуть породу "розовый"</t>
+  </si>
+  <si>
+    <t>Открывается страница с животными породой "розовый", если такие есть в наличии,либо страница с надписью об их отсутствии.</t>
+  </si>
+  <si>
+    <t>Fail Bugs: FB-0011</t>
+  </si>
+  <si>
+    <t>EXP-019</t>
+  </si>
+  <si>
+    <t>Фильтр "пол"</t>
+  </si>
+  <si>
+    <t>1.Кликнуть по фильтру пол.</t>
+  </si>
+  <si>
+    <t>Открывается выпадающий список, в котором корректно указан пол животных и без разных формулировок.</t>
+  </si>
+  <si>
+    <t>Fail Bugs: FB-0012</t>
+  </si>
+  <si>
+    <t>EXP-020</t>
+  </si>
+  <si>
+    <t>Фильтр "возраст"</t>
+  </si>
+  <si>
+    <t>1.Кликнуть по фильтру возраст.
+2.Ввести отрицательное значение</t>
+  </si>
+  <si>
+    <t>Появляется подсказка,что введение отрицательныз значений запрещено.</t>
+  </si>
+  <si>
+    <t>Fail Bugs: FB-0013</t>
+  </si>
+  <si>
+    <t>EXP-021</t>
+  </si>
+  <si>
+    <t>Форма обратной связи
+(внешний вид)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Кликнуть по кнопке "без дома" на карточке питомца.
+</t>
+  </si>
+  <si>
+    <t>В появивщемся окне поля для ввода имеют названия.</t>
+  </si>
+  <si>
+    <t>Fail Bugs: FB-0014</t>
+  </si>
+  <si>
+    <t>EXP-022</t>
+  </si>
+  <si>
+    <t>Форма обратной связи
+(пустая отправка)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Кликнуть по кнопке "без дома" на карточке питомца.
+2.В появившемся окне кликнуть по кнопке "ДА!"
+</t>
+  </si>
+  <si>
+    <t>Появляются подсказки,что поля для вводы не заполнены.</t>
+  </si>
+  <si>
+    <t>EXP-023</t>
+  </si>
+  <si>
+    <t>Форма обратной связи
+(поле введите имя)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Кликнуть по кнопке "без дома" на карточке питомца.
+2.Ввести в поле с подсказкой "введите имя" числовое значение и спец.символ.
+</t>
+  </si>
+  <si>
+    <t>Поле для ввода не принимачает числовые значения и спец.символ,появляется подсказка.</t>
+  </si>
+  <si>
+    <t>Fail Bugs: FB-0015</t>
+  </si>
+  <si>
+    <t>EXP-024</t>
+  </si>
+  <si>
+    <t>Форма обратной связи
+(поле введите фамилию)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Кликнуть по кнопке "без дома" на карточке питомца.
+2.Ввести в поле с подсказкой "введите фамилию" числовое значение спец.символ.
+</t>
+  </si>
+  <si>
+    <t>Fail Bugs: FB-0016</t>
+  </si>
+  <si>
+    <t>EXP-025</t>
+  </si>
+  <si>
+    <t>Форма обратной связи
+(поле введите отчество)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Кликнуть по кнопке "без дома" на карточке питомца.
+2.Ввести в поле с подсказкой "введите отчество" числовое значение спец.символ.
+</t>
+  </si>
+  <si>
+    <t>Fail Bugs: FB-0017</t>
+  </si>
+  <si>
+    <t>EXP-026</t>
+  </si>
+  <si>
+    <t>Форма обратной связи
+(поле +7 ваш номер)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Кликнуть по кнопке "без дома" на карточке питомца.
+2.Введите в поле с подсказкой "+7 ваш номер" номер не соответствующий формату подсказки.
+</t>
+  </si>
+  <si>
+    <t>Появляется подсказка Номер должен соответствовать +79********* !</t>
+  </si>
+  <si>
+    <t>EXP-027</t>
+  </si>
+  <si>
+    <t>Форма обратной связи
+(поле EMAIL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Кликнуть по кнопке "без дома" на карточке питомца.
+2.Введите в поле с подсказкой "your@email.com" ,email не соответствующий формату подскази.
+</t>
+  </si>
+  <si>
+    <t>Появляется подсказка Enter a valid email address.</t>
+  </si>
+  <si>
+    <t>EXP-028</t>
+  </si>
+  <si>
+    <t>Форма обратной связи
+(заполненная отправка)</t>
+  </si>
+  <si>
+    <t>1.Кликнуть по кнопке "без дома" на карточке питомца.
+2.В появившемся окне корректно заполнить все поля для ввода. 
+3.Клинкуть по кнопке "ДА!"</t>
+  </si>
+  <si>
+    <t>Появляется подсказка,что форма обратной связи отправлена.</t>
+  </si>
+  <si>
+    <t>Fail Bugs: FB-0018</t>
   </si>
 </sst>
 </file>
@@ -349,7 +793,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,8 +830,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAEEF3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -462,6 +918,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -470,23 +986,11 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -537,6 +1041,63 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -835,7 +1396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
@@ -849,1167 +1410,1167 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.5">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="7"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" ht="15.5">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="15.5">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="28">
       <c r="A5" s="3"/>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="28">
       <c r="A6" s="3"/>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="28">
       <c r="A7" s="3"/>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:11" ht="56">
       <c r="A8" s="3"/>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:11" ht="42.5" thickBot="1">
       <c r="A9" s="3"/>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:11" ht="42.5" thickBot="1">
       <c r="A10" s="3"/>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="42.5" thickBot="1">
       <c r="A11" s="3"/>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="42.5" thickBot="1">
       <c r="A12" s="3"/>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="42.5" thickBot="1">
       <c r="A13" s="3"/>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="28.5" thickBot="1">
       <c r="A14" s="3"/>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:11" ht="42.5" thickBot="1">
       <c r="A15" s="3"/>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:11" ht="42.5" thickBot="1">
       <c r="A16" s="3"/>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" ht="42.5" thickBot="1">
       <c r="A17" s="3"/>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" ht="28">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3"/>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" ht="56">
       <c r="A20" s="3"/>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" ht="28">
       <c r="A21" s="3"/>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" ht="28">
       <c r="A22" s="3"/>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" ht="49" customHeight="1">
       <c r="A23" s="3"/>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" ht="42">
       <c r="A24" s="3"/>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" ht="42">
       <c r="A25" s="3"/>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" ht="56">
       <c r="A26" s="3"/>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" ht="42">
       <c r="A27" s="3"/>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" ht="42">
       <c r="A28" s="3"/>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" ht="42">
       <c r="A29" s="3"/>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" ht="42">
       <c r="A30" s="3"/>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" ht="56">
       <c r="A31" s="3"/>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" ht="28">
       <c r="A32" s="3"/>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" ht="28">
       <c r="A33" s="3"/>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="3"/>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4" ht="42">
       <c r="A35" s="3"/>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" ht="42">
       <c r="A36" s="3"/>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:4" ht="42">
       <c r="A37" s="3"/>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" ht="28">
       <c r="A38" s="3"/>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:4" ht="28">
       <c r="A39" s="3"/>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:4" ht="42">
       <c r="A40" s="3"/>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:4" ht="42.5" thickBot="1">
       <c r="A41" s="3"/>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:4" ht="57" customHeight="1" thickBot="1">
       <c r="A42" s="3"/>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D42" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="57" customHeight="1" thickBot="1">
       <c r="A43" s="3"/>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D43" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="57" customHeight="1" thickBot="1">
       <c r="A44" s="3"/>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="57" customHeight="1" thickBot="1">
       <c r="A45" s="3"/>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D45" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="57" customHeight="1">
       <c r="A46" s="3"/>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D46" s="9"/>
+      <c r="D46" s="5"/>
     </row>
     <row r="47" spans="1:4" ht="57" customHeight="1">
       <c r="A47" s="3"/>
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D47" s="9"/>
+      <c r="D47" s="5"/>
     </row>
     <row r="48" spans="1:4" ht="57" customHeight="1">
       <c r="A48" s="3"/>
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D48" s="9"/>
+      <c r="D48" s="5"/>
     </row>
     <row r="49" spans="1:4" ht="57" customHeight="1">
       <c r="A49" s="3"/>
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D49" s="9"/>
+      <c r="D49" s="5"/>
     </row>
     <row r="50" spans="1:4" ht="57" customHeight="1">
       <c r="A50" s="3"/>
-      <c r="B50" s="16" t="s">
+      <c r="B50" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D50" s="9"/>
+      <c r="C50" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="5"/>
     </row>
     <row r="51" spans="1:4" ht="57" customHeight="1">
       <c r="A51" s="3"/>
-      <c r="B51" s="16" t="s">
+      <c r="B51" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" s="9"/>
+      <c r="C51" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="5"/>
     </row>
     <row r="52" spans="1:4" ht="57" customHeight="1">
       <c r="A52" s="3"/>
-      <c r="B52" s="16" t="s">
+      <c r="B52" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C52" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="9"/>
+      <c r="C52" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="5"/>
     </row>
     <row r="53" spans="1:4" ht="57" customHeight="1">
       <c r="A53" s="3"/>
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C53" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="9"/>
+      <c r="C53" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="5"/>
     </row>
     <row r="54" spans="1:4" ht="57" customHeight="1" thickBot="1">
       <c r="A54" s="3"/>
-      <c r="B54" s="16" t="s">
+      <c r="B54" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D54" s="9"/>
+      <c r="D54" s="5"/>
     </row>
     <row r="55" spans="1:4" ht="57" customHeight="1" thickBot="1">
       <c r="A55" s="3"/>
-      <c r="B55" s="13" t="s">
+      <c r="B55" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C55" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D55" s="9"/>
+      <c r="C55" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="5"/>
     </row>
     <row r="56" spans="1:4" ht="57" customHeight="1" thickBot="1">
       <c r="A56" s="3"/>
-      <c r="B56" s="13" t="s">
+      <c r="B56" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C56" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D56" s="9"/>
+      <c r="C56" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="5"/>
     </row>
     <row r="57" spans="1:4" ht="57" customHeight="1" thickBot="1">
       <c r="A57" s="3"/>
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C57" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D57" s="9"/>
+      <c r="C57" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" s="5"/>
     </row>
     <row r="58" spans="1:4" ht="28">
-      <c r="A58" s="19" t="s">
+      <c r="A58" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="C58" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D58" s="20"/>
+      <c r="C58" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="16"/>
     </row>
     <row r="59" spans="1:4" ht="56">
-      <c r="A59" s="20"/>
-      <c r="B59" s="10" t="s">
+      <c r="A59" s="16"/>
+      <c r="B59" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D59" s="20"/>
+      <c r="C59" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="16"/>
     </row>
     <row r="60" spans="1:4" ht="28">
-      <c r="A60" s="20"/>
-      <c r="B60" s="15" t="s">
+      <c r="A60" s="16"/>
+      <c r="B60" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D60" s="20"/>
+      <c r="D60" s="16"/>
     </row>
     <row r="61" spans="1:4" ht="42">
-      <c r="A61" s="20"/>
-      <c r="B61" s="9" t="s">
+      <c r="A61" s="16"/>
+      <c r="B61" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C61" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D61" s="20"/>
+      <c r="C61" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="16"/>
     </row>
     <row r="62" spans="1:4" ht="42.5" thickBot="1">
-      <c r="A62" s="20"/>
-      <c r="B62" s="16" t="s">
+      <c r="A62" s="16"/>
+      <c r="B62" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="C62" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D62" s="20"/>
+      <c r="D62" s="16"/>
     </row>
     <row r="63" spans="1:4" ht="42.5" thickBot="1">
-      <c r="A63" s="20"/>
-      <c r="B63" s="13" t="s">
+      <c r="A63" s="16"/>
+      <c r="B63" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C63" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D63" s="20"/>
+      <c r="C63" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="16"/>
     </row>
     <row r="64" spans="1:4" ht="42.5" thickBot="1">
-      <c r="A64" s="20"/>
-      <c r="B64" s="13" t="s">
+      <c r="A64" s="16"/>
+      <c r="B64" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C64" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D64" s="20"/>
+      <c r="C64" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" s="16"/>
     </row>
     <row r="65" spans="1:4" ht="42.5" thickBot="1">
-      <c r="A65" s="20"/>
-      <c r="B65" s="13" t="s">
+      <c r="A65" s="16"/>
+      <c r="B65" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C65" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D65" s="20"/>
+      <c r="C65" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="16"/>
     </row>
     <row r="66" spans="1:4" ht="42.5" thickBot="1">
-      <c r="A66" s="20"/>
-      <c r="B66" s="13" t="s">
+      <c r="A66" s="16"/>
+      <c r="B66" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C66" s="11" t="s">
+      <c r="C66" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D66" s="10" t="s">
+      <c r="D66" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="42.5" thickBot="1">
-      <c r="A67" s="20"/>
-      <c r="B67" s="14" t="s">
+      <c r="A67" s="16"/>
+      <c r="B67" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C67" s="11" t="s">
+      <c r="C67" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D67" s="10" t="s">
+      <c r="D67" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="42.5" thickBot="1">
-      <c r="A68" s="20"/>
-      <c r="B68" s="13" t="s">
+      <c r="A68" s="16"/>
+      <c r="B68" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C68" s="11" t="s">
+      <c r="C68" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D68" s="10" t="s">
+      <c r="D68" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="42.5" thickBot="1">
-      <c r="A69" s="20"/>
-      <c r="B69" s="14" t="s">
+      <c r="A69" s="16"/>
+      <c r="B69" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C69" s="11" t="s">
+      <c r="C69" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D69" s="10" t="s">
+      <c r="D69" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="44" thickBot="1">
-      <c r="A70" s="21" t="s">
+      <c r="A70" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B70" s="24" t="s">
+      <c r="B70" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C70" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D70" s="20"/>
+      <c r="C70" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" s="16"/>
     </row>
     <row r="71" spans="1:4" ht="43.5">
-      <c r="A71" s="20"/>
-      <c r="B71" s="20" t="s">
+      <c r="A71" s="16"/>
+      <c r="B71" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="C71" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D71" s="22" t="s">
+      <c r="D71" s="18" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="42">
-      <c r="A72" s="20"/>
-      <c r="B72" s="20" t="s">
+      <c r="A72" s="16"/>
+      <c r="B72" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C72" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D72" s="20"/>
+      <c r="C72" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" s="16"/>
     </row>
     <row r="73" spans="1:4" ht="42">
-      <c r="A73" s="20"/>
-      <c r="B73" s="20" t="s">
+      <c r="A73" s="16"/>
+      <c r="B73" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C73" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D73" s="20"/>
+      <c r="C73" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" s="16"/>
     </row>
     <row r="74" spans="1:4" ht="43.5">
-      <c r="A74" s="20"/>
-      <c r="B74" s="20" t="s">
+      <c r="A74" s="16"/>
+      <c r="B74" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="C74" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D74" s="22" t="s">
+      <c r="D74" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="42">
-      <c r="A75" s="20"/>
-      <c r="B75" s="20" t="s">
+      <c r="A75" s="16"/>
+      <c r="B75" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C75" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D75" s="20"/>
+      <c r="C75" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" s="16"/>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="23"/>
-      <c r="B76" s="20"/>
-      <c r="C76" s="20"/>
-      <c r="D76" s="20"/>
+      <c r="A76" s="19"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="16"/>
+      <c r="D76" s="16"/>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="20"/>
-      <c r="B77" s="20"/>
-      <c r="C77" s="20"/>
-      <c r="D77" s="20"/>
+      <c r="A77" s="16"/>
+      <c r="B77" s="16"/>
+      <c r="C77" s="16"/>
+      <c r="D77" s="16"/>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="20"/>
-      <c r="B78" s="20"/>
-      <c r="C78" s="20"/>
-      <c r="D78" s="20"/>
+      <c r="A78" s="16"/>
+      <c r="B78" s="16"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="16"/>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="20"/>
-      <c r="B79" s="20"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="20"/>
+      <c r="A79" s="16"/>
+      <c r="B79" s="16"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="16"/>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="20"/>
-      <c r="B80" s="20"/>
-      <c r="C80" s="20"/>
-      <c r="D80" s="20"/>
+      <c r="A80" s="16"/>
+      <c r="B80" s="16"/>
+      <c r="C80" s="16"/>
+      <c r="D80" s="16"/>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="20"/>
-      <c r="B81" s="20"/>
-      <c r="C81" s="20"/>
-      <c r="D81" s="20"/>
+      <c r="A81" s="16"/>
+      <c r="B81" s="16"/>
+      <c r="C81" s="16"/>
+      <c r="D81" s="16"/>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="20"/>
-      <c r="B82" s="20"/>
-      <c r="C82" s="20"/>
-      <c r="D82" s="20"/>
+      <c r="A82" s="16"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="16"/>
+      <c r="D82" s="16"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="20"/>
-      <c r="B83" s="20"/>
-      <c r="C83" s="20"/>
-      <c r="D83" s="20"/>
+      <c r="A83" s="16"/>
+      <c r="B83" s="16"/>
+      <c r="C83" s="16"/>
+      <c r="D83" s="16"/>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="20"/>
-      <c r="B84" s="20"/>
-      <c r="C84" s="20"/>
-      <c r="D84" s="20"/>
+      <c r="A84" s="16"/>
+      <c r="B84" s="16"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="16"/>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="20"/>
-      <c r="B85" s="20"/>
-      <c r="C85" s="20"/>
-      <c r="D85" s="20"/>
+      <c r="A85" s="16"/>
+      <c r="B85" s="16"/>
+      <c r="C85" s="16"/>
+      <c r="D85" s="16"/>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="20"/>
-      <c r="B86" s="20"/>
-      <c r="C86" s="20"/>
-      <c r="D86" s="20"/>
+      <c r="A86" s="16"/>
+      <c r="B86" s="16"/>
+      <c r="C86" s="16"/>
+      <c r="D86" s="16"/>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" s="20"/>
-      <c r="B87" s="20"/>
-      <c r="C87" s="20"/>
-      <c r="D87" s="20"/>
+      <c r="A87" s="16"/>
+      <c r="B87" s="16"/>
+      <c r="C87" s="16"/>
+      <c r="D87" s="16"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="20"/>
-      <c r="B88" s="20"/>
-      <c r="C88" s="20"/>
-      <c r="D88" s="20"/>
+      <c r="A88" s="16"/>
+      <c r="B88" s="16"/>
+      <c r="C88" s="16"/>
+      <c r="D88" s="16"/>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="20"/>
-      <c r="B89" s="20"/>
-      <c r="C89" s="20"/>
-      <c r="D89" s="20"/>
+      <c r="A89" s="16"/>
+      <c r="B89" s="16"/>
+      <c r="C89" s="16"/>
+      <c r="D89" s="16"/>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="20"/>
-      <c r="B90" s="20"/>
-      <c r="C90" s="20"/>
-      <c r="D90" s="20"/>
+      <c r="A90" s="16"/>
+      <c r="B90" s="16"/>
+      <c r="C90" s="16"/>
+      <c r="D90" s="16"/>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="20"/>
-      <c r="B91" s="20"/>
-      <c r="C91" s="20"/>
-      <c r="D91" s="20"/>
+      <c r="A91" s="16"/>
+      <c r="B91" s="16"/>
+      <c r="C91" s="16"/>
+      <c r="D91" s="16"/>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="20"/>
-      <c r="B92" s="20"/>
-      <c r="C92" s="20"/>
-      <c r="D92" s="20"/>
+      <c r="A92" s="16"/>
+      <c r="B92" s="16"/>
+      <c r="C92" s="16"/>
+      <c r="D92" s="16"/>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="20"/>
-      <c r="B93" s="20"/>
-      <c r="C93" s="20"/>
-      <c r="D93" s="20"/>
+      <c r="A93" s="16"/>
+      <c r="B93" s="16"/>
+      <c r="C93" s="16"/>
+      <c r="D93" s="16"/>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="20"/>
-      <c r="B94" s="20"/>
-      <c r="C94" s="20"/>
-      <c r="D94" s="20"/>
+      <c r="A94" s="16"/>
+      <c r="B94" s="16"/>
+      <c r="C94" s="16"/>
+      <c r="D94" s="16"/>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="20"/>
-      <c r="B95" s="20"/>
-      <c r="C95" s="20"/>
-      <c r="D95" s="20"/>
+      <c r="A95" s="16"/>
+      <c r="B95" s="16"/>
+      <c r="C95" s="16"/>
+      <c r="D95" s="16"/>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="20"/>
-      <c r="B96" s="20"/>
-      <c r="C96" s="20"/>
-      <c r="D96" s="20"/>
+      <c r="A96" s="16"/>
+      <c r="B96" s="16"/>
+      <c r="C96" s="16"/>
+      <c r="D96" s="16"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="20"/>
-      <c r="B97" s="20"/>
-      <c r="C97" s="20"/>
-      <c r="D97" s="20"/>
+      <c r="A97" s="16"/>
+      <c r="B97" s="16"/>
+      <c r="C97" s="16"/>
+      <c r="D97" s="16"/>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="20"/>
-      <c r="B98" s="20"/>
-      <c r="C98" s="20"/>
-      <c r="D98" s="20"/>
+      <c r="A98" s="16"/>
+      <c r="B98" s="16"/>
+      <c r="C98" s="16"/>
+      <c r="D98" s="16"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="20"/>
-      <c r="B99" s="20"/>
-      <c r="C99" s="20"/>
-      <c r="D99" s="20"/>
+      <c r="A99" s="16"/>
+      <c r="B99" s="16"/>
+      <c r="C99" s="16"/>
+      <c r="D99" s="16"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="17"/>
-      <c r="B100" s="17"/>
-      <c r="C100" s="17"/>
-      <c r="D100" s="17"/>
+      <c r="A100" s="13"/>
+      <c r="B100" s="13"/>
+      <c r="C100" s="13"/>
+      <c r="D100" s="13"/>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="17"/>
-      <c r="B101" s="17"/>
-      <c r="C101" s="17"/>
-      <c r="D101" s="17"/>
+      <c r="A101" s="13"/>
+      <c r="B101" s="13"/>
+      <c r="C101" s="13"/>
+      <c r="D101" s="13"/>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" s="17"/>
-      <c r="B102" s="17"/>
-      <c r="C102" s="17"/>
-      <c r="D102" s="17"/>
+      <c r="A102" s="13"/>
+      <c r="B102" s="13"/>
+      <c r="C102" s="13"/>
+      <c r="D102" s="13"/>
     </row>
     <row r="103" spans="1:4">
-      <c r="A103" s="17"/>
-      <c r="B103" s="17"/>
-      <c r="C103" s="17"/>
-      <c r="D103" s="17"/>
+      <c r="A103" s="13"/>
+      <c r="B103" s="13"/>
+      <c r="C103" s="13"/>
+      <c r="D103" s="13"/>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="17"/>
-      <c r="B104" s="17"/>
-      <c r="C104" s="17"/>
-      <c r="D104" s="17"/>
+      <c r="A104" s="13"/>
+      <c r="B104" s="13"/>
+      <c r="C104" s="13"/>
+      <c r="D104" s="13"/>
     </row>
     <row r="105" spans="1:4">
-      <c r="A105" s="17"/>
-      <c r="B105" s="17"/>
-      <c r="C105" s="17"/>
-      <c r="D105" s="17"/>
+      <c r="A105" s="13"/>
+      <c r="B105" s="13"/>
+      <c r="C105" s="13"/>
+      <c r="D105" s="13"/>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" s="17"/>
-      <c r="B106" s="17"/>
-      <c r="C106" s="17"/>
-      <c r="D106" s="17"/>
+      <c r="A106" s="13"/>
+      <c r="B106" s="13"/>
+      <c r="C106" s="13"/>
+      <c r="D106" s="13"/>
     </row>
     <row r="107" spans="1:4">
-      <c r="A107" s="17"/>
-      <c r="B107" s="17"/>
-      <c r="C107" s="17"/>
-      <c r="D107" s="17"/>
+      <c r="A107" s="13"/>
+      <c r="B107" s="13"/>
+      <c r="C107" s="13"/>
+      <c r="D107" s="13"/>
     </row>
     <row r="108" spans="1:4">
-      <c r="A108" s="17"/>
-      <c r="B108" s="17"/>
-      <c r="C108" s="17"/>
-      <c r="D108" s="17"/>
+      <c r="A108" s="13"/>
+      <c r="B108" s="13"/>
+      <c r="C108" s="13"/>
+      <c r="D108" s="13"/>
     </row>
     <row r="109" spans="1:4">
-      <c r="A109" s="17"/>
-      <c r="B109" s="17"/>
-      <c r="C109" s="17"/>
-      <c r="D109" s="17"/>
+      <c r="A109" s="13"/>
+      <c r="B109" s="13"/>
+      <c r="C109" s="13"/>
+      <c r="D109" s="13"/>
     </row>
     <row r="110" spans="1:4">
-      <c r="A110" s="17"/>
-      <c r="B110" s="17"/>
-      <c r="C110" s="17"/>
-      <c r="D110" s="17"/>
+      <c r="A110" s="13"/>
+      <c r="B110" s="13"/>
+      <c r="C110" s="13"/>
+      <c r="D110" s="13"/>
     </row>
     <row r="111" spans="1:4">
-      <c r="A111" s="17"/>
-      <c r="B111" s="17"/>
-      <c r="C111" s="17"/>
-      <c r="D111" s="17"/>
+      <c r="A111" s="13"/>
+      <c r="B111" s="13"/>
+      <c r="C111" s="13"/>
+      <c r="D111" s="13"/>
     </row>
     <row r="112" spans="1:4">
-      <c r="A112" s="17"/>
-      <c r="B112" s="17"/>
-      <c r="C112" s="17"/>
-      <c r="D112" s="17"/>
+      <c r="A112" s="13"/>
+      <c r="B112" s="13"/>
+      <c r="C112" s="13"/>
+      <c r="D112" s="13"/>
     </row>
     <row r="113" spans="1:4">
-      <c r="A113" s="17"/>
-      <c r="B113" s="17"/>
-      <c r="C113" s="17"/>
-      <c r="D113" s="17"/>
+      <c r="A113" s="13"/>
+      <c r="B113" s="13"/>
+      <c r="C113" s="13"/>
+      <c r="D113" s="13"/>
     </row>
     <row r="114" spans="1:4">
-      <c r="A114" s="17"/>
-      <c r="B114" s="17"/>
-      <c r="C114" s="17"/>
-      <c r="D114" s="17"/>
+      <c r="A114" s="13"/>
+      <c r="B114" s="13"/>
+      <c r="C114" s="13"/>
+      <c r="D114" s="13"/>
     </row>
     <row r="115" spans="1:4">
-      <c r="A115" s="17"/>
-      <c r="B115" s="17"/>
-      <c r="C115" s="17"/>
-      <c r="D115" s="17"/>
+      <c r="A115" s="13"/>
+      <c r="B115" s="13"/>
+      <c r="C115" s="13"/>
+      <c r="D115" s="13"/>
     </row>
     <row r="116" spans="1:4">
-      <c r="A116" s="17"/>
-      <c r="B116" s="17"/>
-      <c r="C116" s="17"/>
-      <c r="D116" s="17"/>
+      <c r="A116" s="13"/>
+      <c r="B116" s="13"/>
+      <c r="C116" s="13"/>
+      <c r="D116" s="13"/>
     </row>
     <row r="117" spans="1:4">
-      <c r="A117" s="17"/>
-      <c r="B117" s="17"/>
-      <c r="C117" s="17"/>
-      <c r="D117" s="17"/>
+      <c r="A117" s="13"/>
+      <c r="B117" s="13"/>
+      <c r="C117" s="13"/>
+      <c r="D117" s="13"/>
     </row>
     <row r="118" spans="1:4">
-      <c r="A118" s="17"/>
-      <c r="B118" s="17"/>
-      <c r="C118" s="17"/>
-      <c r="D118" s="17"/>
+      <c r="A118" s="13"/>
+      <c r="B118" s="13"/>
+      <c r="C118" s="13"/>
+      <c r="D118" s="13"/>
     </row>
     <row r="119" spans="1:4">
-      <c r="A119" s="17"/>
-      <c r="B119" s="17"/>
-      <c r="C119" s="17"/>
-      <c r="D119" s="17"/>
+      <c r="A119" s="13"/>
+      <c r="B119" s="13"/>
+      <c r="C119" s="13"/>
+      <c r="D119" s="13"/>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="17"/>
-      <c r="B120" s="17"/>
-      <c r="C120" s="17"/>
-      <c r="D120" s="17"/>
+      <c r="A120" s="13"/>
+      <c r="B120" s="13"/>
+      <c r="C120" s="13"/>
+      <c r="D120" s="13"/>
     </row>
     <row r="121" spans="1:4">
-      <c r="A121" s="17"/>
-      <c r="B121" s="17"/>
-      <c r="C121" s="17"/>
-      <c r="D121" s="17"/>
+      <c r="A121" s="13"/>
+      <c r="B121" s="13"/>
+      <c r="C121" s="13"/>
+      <c r="D121" s="13"/>
     </row>
     <row r="122" spans="1:4">
-      <c r="A122" s="17"/>
-      <c r="B122" s="17"/>
-      <c r="C122" s="17"/>
-      <c r="D122" s="17"/>
+      <c r="A122" s="13"/>
+      <c r="B122" s="13"/>
+      <c r="C122" s="13"/>
+      <c r="D122" s="13"/>
     </row>
     <row r="123" spans="1:4">
-      <c r="A123" s="17"/>
-      <c r="B123" s="17"/>
-      <c r="C123" s="17"/>
-      <c r="D123" s="17"/>
+      <c r="A123" s="13"/>
+      <c r="B123" s="13"/>
+      <c r="C123" s="13"/>
+      <c r="D123" s="13"/>
     </row>
     <row r="124" spans="1:4">
-      <c r="A124" s="17"/>
-      <c r="B124" s="17"/>
-      <c r="C124" s="17"/>
-      <c r="D124" s="17"/>
+      <c r="A124" s="13"/>
+      <c r="B124" s="13"/>
+      <c r="C124" s="13"/>
+      <c r="D124" s="13"/>
     </row>
     <row r="125" spans="1:4">
-      <c r="A125" s="17"/>
-      <c r="B125" s="17"/>
-      <c r="C125" s="17"/>
-      <c r="D125" s="17"/>
+      <c r="A125" s="13"/>
+      <c r="B125" s="13"/>
+      <c r="C125" s="13"/>
+      <c r="D125" s="13"/>
     </row>
     <row r="126" spans="1:4">
-      <c r="A126" s="17"/>
-      <c r="B126" s="17"/>
-      <c r="C126" s="17"/>
-      <c r="D126" s="17"/>
+      <c r="A126" s="13"/>
+      <c r="B126" s="13"/>
+      <c r="C126" s="13"/>
+      <c r="D126" s="13"/>
     </row>
     <row r="127" spans="1:4">
-      <c r="A127" s="17"/>
-      <c r="B127" s="17"/>
-      <c r="C127" s="17"/>
-      <c r="D127" s="17"/>
+      <c r="A127" s="13"/>
+      <c r="B127" s="13"/>
+      <c r="C127" s="13"/>
+      <c r="D127" s="13"/>
     </row>
     <row r="128" spans="1:4">
-      <c r="A128" s="17"/>
-      <c r="B128" s="17"/>
-      <c r="C128" s="17"/>
-      <c r="D128" s="17"/>
+      <c r="A128" s="13"/>
+      <c r="B128" s="13"/>
+      <c r="C128" s="13"/>
+      <c r="D128" s="13"/>
     </row>
     <row r="129" spans="1:4">
-      <c r="A129" s="17"/>
-      <c r="B129" s="17"/>
-      <c r="C129" s="17"/>
-      <c r="D129" s="17"/>
+      <c r="A129" s="13"/>
+      <c r="B129" s="13"/>
+      <c r="C129" s="13"/>
+      <c r="D129" s="13"/>
     </row>
     <row r="130" spans="1:4">
-      <c r="A130" s="17"/>
-      <c r="B130" s="17"/>
-      <c r="C130" s="17"/>
-      <c r="D130" s="17"/>
+      <c r="A130" s="13"/>
+      <c r="B130" s="13"/>
+      <c r="C130" s="13"/>
+      <c r="D130" s="13"/>
     </row>
     <row r="131" spans="1:4">
-      <c r="A131" s="17"/>
-      <c r="B131" s="17"/>
-      <c r="C131" s="17"/>
-      <c r="D131" s="17"/>
+      <c r="A131" s="13"/>
+      <c r="B131" s="13"/>
+      <c r="C131" s="13"/>
+      <c r="D131" s="13"/>
     </row>
     <row r="132" spans="1:4">
-      <c r="A132" s="17"/>
-      <c r="B132" s="17"/>
-      <c r="C132" s="17"/>
-      <c r="D132" s="17"/>
+      <c r="A132" s="13"/>
+      <c r="B132" s="13"/>
+      <c r="C132" s="13"/>
+      <c r="D132" s="13"/>
     </row>
     <row r="133" spans="1:4">
-      <c r="A133" s="17"/>
-      <c r="B133" s="17"/>
-      <c r="C133" s="17"/>
-      <c r="D133" s="17"/>
+      <c r="A133" s="13"/>
+      <c r="B133" s="13"/>
+      <c r="C133" s="13"/>
+      <c r="D133" s="13"/>
     </row>
     <row r="134" spans="1:4">
-      <c r="A134" s="17"/>
-      <c r="B134" s="17"/>
-      <c r="C134" s="17"/>
-      <c r="D134" s="17"/>
+      <c r="A134" s="13"/>
+      <c r="B134" s="13"/>
+      <c r="C134" s="13"/>
+      <c r="D134" s="13"/>
     </row>
     <row r="135" spans="1:4">
-      <c r="A135" s="17"/>
-      <c r="B135" s="17"/>
-      <c r="C135" s="17"/>
-      <c r="D135" s="17"/>
+      <c r="A135" s="13"/>
+      <c r="B135" s="13"/>
+      <c r="C135" s="13"/>
+      <c r="D135" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2029,12 +2590,708 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="23.08984375" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1">
+      <c r="A1" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="112.5" thickBot="1">
+      <c r="A2" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="29"/>
+      <c r="E2" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="39" customFormat="1" ht="154.5" thickBot="1">
+      <c r="A3" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="112.5" thickBot="1">
+      <c r="A4" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="112.5" thickBot="1">
+      <c r="A5" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="70.5" thickBot="1">
+      <c r="A6" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="112.5" thickBot="1">
+      <c r="A7" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="56.5" thickBot="1">
+      <c r="A8" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="98.5" thickBot="1">
+      <c r="A9" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="70.5" thickBot="1">
+      <c r="A10" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="70.5" thickBot="1">
+      <c r="A11" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="98.5" thickBot="1">
+      <c r="A12" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="70.5" thickBot="1">
+      <c r="A13" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="56.5" thickBot="1">
+      <c r="A14" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="56.5" thickBot="1">
+      <c r="A15" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="56.5" thickBot="1">
+      <c r="A16" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="56.5" thickBot="1">
+      <c r="A17" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="84.5" thickBot="1">
+      <c r="A18" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="98.5" thickBot="1">
+      <c r="A19" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="84.5" thickBot="1">
+      <c r="A20" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="84.5" thickBot="1">
+      <c r="A21" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="70.5" thickBot="1">
+      <c r="A22" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="G22" s="34" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="56.5" thickBot="1">
+      <c r="A23" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="98.5" thickBot="1">
+      <c r="A24" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="F24" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="G24" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="126.5" thickBot="1">
+      <c r="A25" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="F25" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="G25" s="34" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="126.5" thickBot="1">
+      <c r="A26" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="F26" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="G26" s="34" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="126.5" thickBot="1">
+      <c r="A27" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="F27" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="G27" s="34" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="126.5" thickBot="1">
+      <c r="A28" s="33" t="s">
+        <v>211</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="F28" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="G28" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="140.5" thickBot="1">
+      <c r="A29" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>217</v>
+      </c>
+      <c r="F29" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="G29" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="126.5" thickBot="1">
+      <c r="A30" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="F30" s="30" t="s">
+        <v>222</v>
+      </c>
+      <c r="G30" s="34" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
 </worksheet>
@@ -2042,12 +3299,708 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.36328125" customWidth="1"/>
+    <col min="2" max="2" width="13.90625" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="4" max="4" width="17.08984375" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" customWidth="1"/>
+    <col min="6" max="6" width="18.90625" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1">
+      <c r="A1" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="126.5" thickBot="1">
+      <c r="A2" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="29"/>
+      <c r="E2" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="182.5" thickBot="1">
+      <c r="A3" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="140.5" thickBot="1">
+      <c r="A4" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="140.5" thickBot="1">
+      <c r="A5" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="98.5" thickBot="1">
+      <c r="A6" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="154.5" thickBot="1">
+      <c r="A7" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="70.5" thickBot="1">
+      <c r="A8" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="126.5" thickBot="1">
+      <c r="A9" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="84.5" thickBot="1">
+      <c r="A10" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="84.5" thickBot="1">
+      <c r="A11" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="112.5" thickBot="1">
+      <c r="A12" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="112.5" thickBot="1">
+      <c r="A13" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="56.5" thickBot="1">
+      <c r="A14" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="56.5" thickBot="1">
+      <c r="A15" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="56.5" thickBot="1">
+      <c r="A16" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="56.5" thickBot="1">
+      <c r="A17" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="112.5" thickBot="1">
+      <c r="A18" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="126.5" thickBot="1">
+      <c r="A19" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="126.5" thickBot="1">
+      <c r="A20" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="98.5" thickBot="1">
+      <c r="A21" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="84.5" thickBot="1">
+      <c r="A22" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="G22" s="34" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="70.5" thickBot="1">
+      <c r="A23" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="112.5" thickBot="1">
+      <c r="A24" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="F24" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="G24" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="140.5" thickBot="1">
+      <c r="A25" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="F25" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="G25" s="34" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="154.5" thickBot="1">
+      <c r="A26" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="F26" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="G26" s="34" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="140.5" thickBot="1">
+      <c r="A27" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="F27" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="G27" s="34" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="168.5" thickBot="1">
+      <c r="A28" s="33" t="s">
+        <v>211</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="F28" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="G28" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="154.5" thickBot="1">
+      <c r="A29" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>217</v>
+      </c>
+      <c r="F29" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="G29" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="140.5" thickBot="1">
+      <c r="A30" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="F30" s="30" t="s">
+        <v>222</v>
+      </c>
+      <c r="G30" s="34" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
 </worksheet>

</xml_diff>